<commit_message>
function all concept clear
</commit_message>
<xml_diff>
--- a/pythonconcepts.xlsx
+++ b/pythonconcepts.xlsx
@@ -5,18 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\study_hub\python\mayur_practice_python_topicvise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\study_hub\python\git_mayur_practice_python_topicvise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C32D580-FB15-4AE1-B171-21D0DD0313CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7EB260-4508-4155-AE7D-B60CA5749A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tuple" sheetId="1" r:id="rId1"/>
     <sheet name="set" sheetId="2" r:id="rId2"/>
     <sheet name="dictionary" sheetId="3" r:id="rId3"/>
     <sheet name="list" sheetId="4" r:id="rId4"/>
+    <sheet name="function" sheetId="5" r:id="rId5"/>
+    <sheet name="if else and if elif else " sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="138">
   <si>
     <t>tuple are use store multiple items in single variable</t>
   </si>
@@ -601,6 +603,147 @@
   <si>
     <t xml:space="preserve">[4, 6, 10, 26, 30, 40, 80]
 80 40 30 26 10 6 4 </t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A function is block o code wich only runs when it  called.
+you can pass parameter to function
+function car retun data as a result
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">syntax </t>
+  </si>
+  <si>
+    <t>Parameters or Arguments?</t>
+  </si>
+  <si>
+    <t>information pass to function is called parameter or argument</t>
+  </si>
+  <si>
+    <t>Arbitrary Arguments, *args</t>
+  </si>
+  <si>
+    <t># # A parameter is the variable listed inside the parentheses in the function definition.
+# def fun2(x):            # x is called parameter
+#     pass
+# An argument is the value that is sent to the function when it is called.
+# fun2(50)    # 50 is called argument</t>
+  </si>
+  <si>
+    <t>you don’t know how many argument pass to the function then put * infront of parameter</t>
+  </si>
+  <si>
+    <t>def fun4(*par):
+    for x in par:
+        print(x)
+fun4(2,4,5,6)</t>
+  </si>
+  <si>
+    <t>Arbitrary Keyword Arguments, **kwargs</t>
+  </si>
+  <si>
+    <t>you don’t know how many argument key value pass to the function then put ** infront of parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># def fun5(**child):
+#     print(child["child1"])
+# fun5(child1="A",child2="B",child3="c")
+</t>
+  </si>
+  <si>
+    <t>"A"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2
+4
+5
+6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># syntax
+def function_name():
+    print("Hello this is syntax for define the function")
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello this is syntax for define the function  </t>
+  </si>
+  <si>
+    <t>#here you call the function  
+function_name()</t>
+  </si>
+  <si>
+    <t>If we call the function without argument, it uses the default value:</t>
+  </si>
+  <si>
+    <t>Default Parameter Value</t>
+  </si>
+  <si>
+    <t># Default Parameter Value
+def fun6(name = "mayur"):
+    print("Hello",name)
+fun6()
+fun6("rushikesh")</t>
+  </si>
+  <si>
+    <t>Hello mayur
+Hello rushikesh</t>
+  </si>
+  <si>
+    <t>theory</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Passing a List as an Argument</t>
+  </si>
+  <si>
+    <t>You can send any data types of argument to a function (string, number, list, dictionary etc.), and it will be treated as the same data type inside the function.</t>
+  </si>
+  <si>
+    <t>The pass Statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list1 = [1,2,3,4,5]
+tup1=(1,2,3,4,5)
+set1 = {1,2,3,4,5}
+def fun7(l):
+    for x in l:
+        print(x,end=" ")
+    print()
+fun7(list1)
+fun7(tup1)
+fun7(set1)
+dic = {"name":"mayur","last":"baviskar"}
+def fun7(l):
+    for x in l.items():
+        print(x,end=" ")
+    print()
+fun7(dic)
+</t>
+  </si>
+  <si>
+    <t>for define empty function we use pass statement</t>
+  </si>
+  <si>
+    <t># # pass keyword
+# # to define the empty function
+# def fun8():
+#     pass</t>
+  </si>
+  <si>
+    <t>if else</t>
   </si>
 </sst>
 </file>
@@ -709,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -737,6 +880,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -746,23 +907,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,7 +1220,7 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="17" t="s">
         <v>103</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1075,7 +1233,7 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +1244,7 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1097,7 +1255,7 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1269,49 +1427,49 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1319,7 +1477,7 @@
       </c>
     </row>
     <row r="11" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1327,7 +1485,7 @@
       </c>
     </row>
     <row r="12" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1335,7 +1493,7 @@
       </c>
     </row>
     <row r="13" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1343,7 +1501,7 @@
       </c>
     </row>
     <row r="14" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1351,7 +1509,7 @@
       </c>
     </row>
     <row r="15" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1359,7 +1517,7 @@
       </c>
     </row>
     <row r="16" spans="2:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1467,7 +1625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D4D720-C2D9-4654-871F-3192D4488735}">
   <dimension ref="B3:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1624,7 +1782,7 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="2:5" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1634,10 +1792,10 @@
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="2:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="16" t="s">
         <v>92</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -1648,7 +1806,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="14" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1659,7 +1817,7 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="14" t="s">
         <v>99</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1673,4 +1831,164 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A43A71D-B943-4731-96FF-B0FF3CFE6535}">
+  <dimension ref="B2:E10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="54.109375" style="22" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="2:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="2:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="288" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA28633-CF00-4199-B6BE-190C11D1E2A6}">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.21875" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>